<commit_message>
Check en los íconos de Agregar
</commit_message>
<xml_diff>
--- a/0-varios/1. Backup/Catálogo.xlsx
+++ b/0-varios/1. Backup/Catálogo.xlsx
@@ -5,21 +5,21 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Documents\8. ELC\1. Películas\3. Contenido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Documents\1. Proyectos Web\ELC-Peliculas\0-varios\1. Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21570" windowHeight="5490" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21570" windowHeight="5490"/>
   </bookViews>
   <sheets>
-    <sheet name="Década" sheetId="4" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="6" r:id="rId2"/>
-    <sheet name="BD" sheetId="1" r:id="rId3"/>
+    <sheet name="BD" sheetId="1" r:id="rId1"/>
+    <sheet name="Década" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId3"/>
     <sheet name="Resumen" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">BD!$A$1:$K$133</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">BD!$1:$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BD!$A$1:$K$133</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">BD!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
@@ -4785,296 +4785,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>1935</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>1940</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>1945</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>1950</v>
-      </c>
-      <c r="B8" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>1955</v>
-      </c>
-      <c r="B9" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>1960</v>
-      </c>
-      <c r="B10" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>1965</v>
-      </c>
-      <c r="B11" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>1970</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>1975</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>1980</v>
-      </c>
-      <c r="B14" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>1985</v>
-      </c>
-      <c r="B15" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
-        <v>1990</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>1995</v>
-      </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>2000</v>
-      </c>
-      <c r="B18" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>2005</v>
-      </c>
-      <c r="B19" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>2010</v>
-      </c>
-      <c r="B20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B21" s="5">
-        <v>89</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B4" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B6" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B7" s="5">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="B8" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="B9" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="B10" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B11" s="5">
-        <v>89</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3" filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
     </sheetView>
@@ -9436,11 +9152,295 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja2"/>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1935</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>1940</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1945</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1950</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>1955</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>1960</v>
+      </c>
+      <c r="B10" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>1965</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>1970</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>1975</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>1980</v>
+      </c>
+      <c r="B14" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>1985</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>1990</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>1995</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>2000</v>
+      </c>
+      <c r="B18" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>2005</v>
+      </c>
+      <c r="B19" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" s="5">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B9" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="5">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F425"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Avances en Detalle de producto
</commit_message>
<xml_diff>
--- a/0-varios/1. Backup/Catálogo.xlsx
+++ b/0-varios/1. Backup/Catálogo.xlsx
@@ -4785,14 +4785,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja3" filterMode="1">
+  <sheetPr codeName="Hoja3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4846,7 +4846,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>64</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>64</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>64</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>64</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>64</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>64</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>64</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
@@ -5841,7 +5841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>64</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>64</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>64</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>64</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>64</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>64</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>64</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>64</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>64</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>64</v>
       </c>
@@ -6516,7 +6516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>64</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>64</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>64</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>64</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>64</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>64</v>
       </c>
@@ -6732,7 +6732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>64</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>64</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>64</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>64</v>
       </c>
@@ -7059,7 +7059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>64</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>64</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>64</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>64</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>64</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>64</v>
       </c>
@@ -7508,7 +7508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>64</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>64</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>64</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>64</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>64</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>64</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>64</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>64</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>64</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>64</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>64</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>64</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>64</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>64</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>64</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>64</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>82</v>
       </c>
@@ -8082,7 +8082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>82</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>82</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>82</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>266</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>266</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>266</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>266</v>
       </c>
@@ -8288,7 +8288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>266</v>
       </c>
@@ -8349,7 +8349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>266</v>
       </c>
@@ -8375,7 +8375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>266</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>266</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>266</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>266</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>266</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>266</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>266</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>266</v>
       </c>
@@ -8581,7 +8581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>266</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>266</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>266</v>
       </c>
@@ -8650,7 +8650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>266</v>
       </c>
@@ -8673,7 +8673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>266</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>266</v>
       </c>
@@ -8719,7 +8719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>266</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>266</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>266</v>
       </c>
@@ -8794,7 +8794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>266</v>
       </c>
@@ -8817,7 +8817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>266</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>266</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>266</v>
       </c>
@@ -8886,7 +8886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>266</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>266</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>266</v>
       </c>
@@ -8958,7 +8958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>266</v>
       </c>
@@ -8981,7 +8981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>266</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>266</v>
       </c>
@@ -9030,7 +9030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>266</v>
       </c>
@@ -9053,7 +9053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>266</v>
       </c>
@@ -9076,7 +9076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>266</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>266</v>
       </c>
@@ -9123,20 +9123,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K133">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Crónica de un hombre santo"/>
-        <filter val="Edison, el hombre"/>
-        <filter val="Forja de hombres"/>
-        <filter val="Karol, el hombre que se convirtió en Papa"/>
-        <filter val="Un hombre para la eternidad"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:K133">
-      <sortCondition ref="I96"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:K133"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E72" r:id="rId1" display="http://www.imdb.com/name/nm0863254/?ref_=tt_ov_dr"/>

</xml_diff>